<commit_message>
Issue #1 work done, needs testing to verify..
</commit_message>
<xml_diff>
--- a/Dev Resources/IO Standards VIVADO.xlsx
+++ b/Dev Resources/IO Standards VIVADO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git Projects\CMOD A7 Artix 7 Isolator V1\CMOD-A7-Artix-7-Buffer-Board\Dev Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B8DD9DC-DB60-4FFA-8F38-1263AB8F3EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D5BAAC-4872-4058-BAD4-C188DB4BFE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="615" windowWidth="28800" windowHeight="15435" xr2:uid="{E9844FC7-4CC0-4DC0-9E88-FF394065EE7A}"/>
+    <workbookView xWindow="9450" yWindow="1875" windowWidth="28800" windowHeight="15435" xr2:uid="{E9844FC7-4CC0-4DC0-9E88-FF394065EE7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
   <si>
     <t>IO Standards</t>
   </si>
@@ -96,14 +96,91 @@
   </si>
   <si>
     <t>PCI33_3</t>
+  </si>
+  <si>
+    <t>A+B</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>B Side Only</t>
+  </si>
+  <si>
+    <t>Supplies needed (Want)</t>
+  </si>
+  <si>
+    <t>Buffer Side (Want)</t>
+  </si>
+  <si>
+    <t>TXB0108 Limits</t>
+  </si>
+  <si>
+    <t>A: 1.2V - 3.6V</t>
+  </si>
+  <si>
+    <t>B: 1.65V - 5.5V</t>
+  </si>
+  <si>
+    <t>Will Make (A)</t>
+  </si>
+  <si>
+    <t>Will Make (B)</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Must always: A &lt; B</t>
+  </si>
+  <si>
+    <t>B &gt; A make circuit to ensure</t>
+  </si>
+  <si>
+    <t>NCV8164</t>
+  </si>
+  <si>
+    <t>VO</t>
+  </si>
+  <si>
+    <t>VREF</t>
+  </si>
+  <si>
+    <t>R1 Val</t>
+  </si>
+  <si>
+    <t>R2 Cal</t>
+  </si>
+  <si>
+    <t>~8k</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~10k</t>
+  </si>
+  <si>
+    <t>~6k65</t>
+  </si>
+  <si>
+    <t>~4k78</t>
+  </si>
+  <si>
+    <t>~3k62</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -131,9 +208,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,18 +527,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA02E51-6392-4B53-9EBF-122B02CB1303}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -475,7 +559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -483,7 +567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -491,7 +575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -499,7 +583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -507,7 +591,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -515,7 +599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -523,7 +607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -531,7 +615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -539,7 +623,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -547,7 +631,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -555,7 +639,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -563,7 +647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -571,12 +655,241 @@
         <v>16</v>
       </c>
     </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>10000</v>
+      </c>
+      <c r="D25">
+        <v>1.2</v>
+      </c>
+      <c r="E25">
+        <f>(C27*C25)/D25-C27</f>
+        <v>9998.7999999999993</v>
+      </c>
+      <c r="F25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26">
+        <v>1.5</v>
+      </c>
+      <c r="E26">
+        <f>(C27*C25)/D26-C27</f>
+        <v>7998.8</v>
+      </c>
+      <c r="F26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="D27">
+        <v>1.8</v>
+      </c>
+      <c r="E27">
+        <f>(C27*C25)/D27-C27</f>
+        <v>6665.4666666666662</v>
+      </c>
+      <c r="F27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>2.5</v>
+      </c>
+      <c r="E28">
+        <f>(C27*C25)/D28-C27</f>
+        <v>4798.8</v>
+      </c>
+      <c r="F28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>3.3</v>
+      </c>
+      <c r="E29">
+        <f>(C27*C25)/D29-C27</f>
+        <v>3635.1636363636367</v>
+      </c>
+      <c r="F29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <f>(C27*C25)/D30-C27</f>
+        <v>2398.8000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101006F85EDBD98026947A6F2DD5CFB3F67C3" ma:contentTypeVersion="7" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="c6ed692721d39106c62d28a0c3244b83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="832ab30c-87f5-4d0a-ad1d-6e51e408aba9" xmlns:ns4="dbc297f8-5430-42f7-9869-539392fb8735" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="de24b102ec5e87e25e310b146bf8c145" ns3:_="" ns4:_="">
     <xsd:import namespace="832ab30c-87f5-4d0a-ad1d-6e51e408aba9"/>
@@ -761,22 +1074,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83DFC7AA-915D-4454-B36D-5DD5BFD026DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="832ab30c-87f5-4d0a-ad1d-6e51e408aba9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="dbc297f8-5430-42f7-9869-539392fb8735"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{130ABF19-7064-40B5-897D-99F6DDFAB9F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{268DEEC7-AC63-4819-9490-8F904C5DF6D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -793,29 +1116,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{130ABF19-7064-40B5-897D-99F6DDFAB9F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83DFC7AA-915D-4454-B36D-5DD5BFD026DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="832ab30c-87f5-4d0a-ad1d-6e51e408aba9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="dbc297f8-5430-42f7-9869-539392fb8735"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>